<commit_message>
Add get mp3 file project and change for new requirement
Thêm project để get audio file, chỉnh sửa lại file audio, theo yêu cầu mới, file .docx
</commit_message>
<xml_diff>
--- a/NewAudio/Audio.xlsx
+++ b/NewAudio/Audio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\Audio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\NewAudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826219EE-4827-4419-9AD8-4AA3FD083154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F15BB0-B086-4B9D-AF8D-87EC897942B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +310,18 @@
   </si>
   <si>
     <t>Sau 30p</t>
+  </si>
+  <si>
+    <t>27/09</t>
+  </si>
+  <si>
+    <t>Chào mừng bạn đến với máy tập thông minh Hec Quyn. Bạn hãy dành 30 giây để nghe Huấn luyện viên Sport One hướng dẫn cách sử dụng máy.Phím start để bắt đầu. Phím Stốp để dừng lại. Nhấn và giữ phím Stốp 3 giây để tắt hoặc bật chế độ huấn luyện viên. Phím Program để chọn 1 trong 12 bài tập mặc định sẵn, máy tự động tăng giảm tốc độ và độ dốc trong khoảng thời gian 30 phút, chú ý những bài tập này thường dùng cho người tập quen. Phím Mode để bạn lựa chọn cài đặt như: thời gian ,khoảng cách  ,calo tiêu hao. Trước khi bắt đầu chạy bạn nên đi giày và dành khoảng 5 phút để khởi động bằng các chức năng đã tích hợp trên máynhư xoay eo,gập bụng. Bạn hãy khởi động cùng tôi nhé: 
+Xoay eo: bạn để bàn xoay xuống đất cạnh đầu máy tập, chân đứng chữ V trên bàn xoay, tay bám lên tay cầm của máy rồi xoay từ phải qua trái và ngược lại. chú ý: khi xoay  giữ nguyên vai chỉ chuyển động phần thân dưới.Xoay 15 đến 20 cái trong 1 hiệp, nên xoay từ 3 đến 5 hiệp.
+Gập bụng: 2 chân để vào giữa mút xốp của hai thanh thép ngang trên đầu máy, chân để trùng, lưng cong, ngả xuống hít sâu, gập lên thở ra.Gập 15 đến 20 cái trong 1 hiệp,Bạn nên  tập từ 3 đến 5 hiệp.
+Bây giờ bạn vào bài tập chạy cùng tôi nhé.
+Bước 1: Đầu tiên bạn cài khóa an toàn vào áo.
+Bước 2: Tay trái bạn đặt lên tay cầm của máy, tay phải ấn nút Start rồi đặt cả 2 tay lên tay cầm của máy.
+Bước 3: Với thời gian tập trung bình 20 đến 30 phút mỗi lần, 5 phút đầu bạn đi bộ và ấn nút Speed cộng để tăng tốc độ với vận tốc từ 1 đến 5 kilomet trên giờ để làm nóng cơ thể.Bạn có thể theo dõi các thông số như vận tốc, quãng đường, nhịp tim, lượng calo độ dốc trên màn hình</t>
   </si>
 </sst>
 </file>
@@ -331,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -363,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -389,7 +407,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,11 +696,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,13 +708,14 @@
     <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="73.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="62.28515625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="73.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="57.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="63.5703125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="81.5703125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,11 +731,14 @@
       <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -726,11 +754,14 @@
       <c r="E2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="G2" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -743,11 +774,11 @@
       <c r="D3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -759,7 +790,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -771,7 +802,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -783,7 +814,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -795,7 +826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -809,11 +840,11 @@
       <c r="E8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -825,7 +856,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -837,7 +868,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -849,7 +880,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -861,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -873,7 +904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -885,7 +916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -897,7 +928,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -959,7 +990,7 @@
       <c r="E20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1061,7 +1092,7 @@
       <c r="E28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1118,7 +1149,7 @@
       <c r="E32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1132,7 +1163,7 @@
       <c r="C33" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1146,7 +1177,7 @@
       <c r="C34" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="11" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1160,7 +1191,7 @@
       <c r="C35" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="9" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bat tat remind cho k bi noi de len nhau V1
</commit_message>
<xml_diff>
--- a/NewAudio/Audio.xlsx
+++ b/NewAudio/Audio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\NewAudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F15BB0-B086-4B9D-AF8D-87EC897942B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974E9D6E-8E2E-48BB-840E-118C3E84DEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>27/09</t>
+  </si>
+  <si>
+    <t>Bước 3: Với thời gian tập trung bình 20 đến 30 phút mỗi lần, 5 phút đầu bạn đi bộ và ấn nút Speed cộng để tăng tốc độ với vận tốc từ 1 đến 5 kilomet trên giờ để làm nóng cơ thể.Bạn có thể theo dõi các thông số như vận tốc, quãng đường, nhịp tim, lượng calo độ dốc trên màn hình</t>
   </si>
   <si>
     <t>Chào mừng bạn đến với máy tập thông minh Hec Quyn. Bạn hãy dành 30 giây để nghe Huấn luyện viên Sport One hướng dẫn cách sử dụng máy.Phím start để bắt đầu. Phím Stốp để dừng lại. Nhấn và giữ phím Stốp 3 giây để tắt hoặc bật chế độ huấn luyện viên. Phím Program để chọn 1 trong 12 bài tập mặc định sẵn, máy tự động tăng giảm tốc độ và độ dốc trong khoảng thời gian 30 phút, chú ý những bài tập này thường dùng cho người tập quen. Phím Mode để bạn lựa chọn cài đặt như: thời gian ,khoảng cách  ,calo tiêu hao. Trước khi bắt đầu chạy bạn nên đi giày và dành khoảng 5 phút để khởi động bằng các chức năng đã tích hợp trên máynhư xoay eo,gập bụng. Bạn hãy khởi động cùng tôi nhé: 
@@ -320,8 +323,58 @@
 Gập bụng: 2 chân để vào giữa mút xốp của hai thanh thép ngang trên đầu máy, chân để trùng, lưng cong, ngả xuống hít sâu, gập lên thở ra.Gập 15 đến 20 cái trong 1 hiệp,Bạn nên  tập từ 3 đến 5 hiệp.
 Bây giờ bạn vào bài tập chạy cùng tôi nhé.
 Bước 1: Đầu tiên bạn cài khóa an toàn vào áo.
-Bước 2: Tay trái bạn đặt lên tay cầm của máy, tay phải ấn nút Start rồi đặt cả 2 tay lên tay cầm của máy.
-Bước 3: Với thời gian tập trung bình 20 đến 30 phút mỗi lần, 5 phút đầu bạn đi bộ và ấn nút Speed cộng để tăng tốc độ với vận tốc từ 1 đến 5 kilomet trên giờ để làm nóng cơ thể.Bạn có thể theo dõi các thông số như vận tốc, quãng đường, nhịp tim, lượng calo độ dốc trên màn hình</t>
+Bước 2: Tay trái bạn đặt lên tay cầm của máy, tay phải ấn nút Start rồi đặt cả 2 tay lên tay cầm của máy.</t>
+  </si>
+  <si>
+    <t>Bước 4: Với khoảng 10 phút tiếp theo bạn ấn phím Speed cộng để tăng lên tốc độ từ 5 đến 7 km trên giờ để chạy chậm , từ 7 đến 9 km trên giờ để chạy trung bình  . Để tăng độ khó và đốt nhiều hơn calo bạn hãy ấn nút mũi tên lên Incline bên trái để nâng độ dốc. Khi chạy mắt nhìn thẳng về phía trước, lưng thẳng , 2 tay co vuông góc đánh theo nhịp bước chân, khi chạy một nửa bàn chân trước tiếp xúc với bàn chạy, luôn giữ nhịp thở đều</t>
+  </si>
+  <si>
+    <t>Bước 5: Với khoảng 5 phút tiếp theo bạn có thể sử dụng phím Speed cộng để thay đổi tốc độ chạy nhanh từ 9 đến 14 kilomet trên giờ để đốt calo nhiều hơn, bạn luôn giữ hơi thở đều để không ảnh hưởng đến nhịp tim , nếu bạn cảm thấy mệt, hơi thở gấp hãy ấn nút speed trừ để giảm tốc độ cho phù hợp</t>
+  </si>
+  <si>
+    <t>Sau 20p</t>
+  </si>
+  <si>
+    <t>Bước 6: Với khoảng 5 đến 10 phút tiếp theo bạn có thể sử dụng phím Speed trừ và mũi tên xuống incline bên phải để giảm độ dốc và tốc độ cho phù hợp cơ thể không bị dừng vận động đột ngột</t>
+  </si>
+  <si>
+    <t>Bước 7: Bạn hãy ấn nút Stop để kết thức bài tập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chúc mừng bạn đã hoàn thành buổi tập . Bạn không nên ngồi xuống ngay hãy đi lại nhẹ nhàng và hít thở đều
+Bước 8. Bạn sử dụng máy mát xa năm đến mười phút để thả lỏng cơ bằng cách khoác dây đai mát xa vào người và ấn công tắc mở để bắt đâu mát xa, di chuyển dây đai mát xa đến các vị trí như bụng ,lưng vai gáy , mông đùi, mỗi vị trí mát xa khoảng một phút rồi di chuyển dây đai đến vị trí khác .
+Bước 9. Khi tập luyện xong bạn nên uống nước lọc ,không lên uống nước có ga . Chú ý: khi uống nước theo ngụm nhỏ uống từ từ , không lên uống nhanh.
+• Với 30 phút tập luyện mỗi ngày bạn sẽ có một dáng vóc hoàng hảo, đặc biệt tốt cho hệ tim mạch, tăng cường trao đổi chất, giúp cơ thể cải thiện hệ thống xương khớp, tăng sự dẻo dai cho cơ thể.
+• Nếu bạn là một chuyên gia thường xuyên luyện tập có thể bỏ qua chức năng Huấn luyện viên để quan tâm đến các chức năng theo dõi tim mạch calo bằng cách nhấn nút Stop 3 giây khi khởi động máy.
+Với máy tập thông minh Hec Quyn bạn sẽ có trải nghiệm tập như chơi, dáng tuyệt vời. Cảm ơn bạn đã sử dụng tôi. Hẹn bạn vào buổi tập tiếp theo nhé.
+</t>
+  </si>
+  <si>
+    <t>luôn giữ hơi thở đều để không ảnh hưởng đến nhịp tim , nếu bạn cảm thấy mệt, hơi thở gấp hãy ấn nút speed trừ để giảm tốc độ cho phù hợp</t>
+  </si>
+  <si>
+    <t>Sau 5 phút đầu tiên, cứ 2 phút nhắc 1 lần</t>
+  </si>
+  <si>
+    <t>Sau khi lắp lại khóa an toàn</t>
+  </si>
+  <si>
+    <t>Lời chào sau khi lắp lại khóa an toàn</t>
+  </si>
+  <si>
+    <t>Khi tháo khóa an toàn</t>
+  </si>
+  <si>
+    <t>5 phút đầu tiên, nhắc tăng tốc sau 30s</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>Bạn hãy ấn nút Speed cộng để tăng dần tốc độ, nên bước đều chân ,thẳng lưng, mắt nhìn thẳng hướng về phía trước,lấy hơi thở đều để không ảnh hưởng đến nhịp tim, nếu bạn cảm thấy mệt, hơi thở gấp hãy ấn nút speed trừ để giảm tốc độ cho phù hợp</t>
   </si>
 </sst>
 </file>
@@ -343,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +421,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -381,14 +440,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -415,6 +468,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,593 +769,614 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="73.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="57.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="63.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="81.5703125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="81.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="360" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="375" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="C25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="C29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B30" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="B31" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="B32" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="B33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
+      <c r="B35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="B36" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>34</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>35</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>36</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C48" s="5"/>
+      <c r="C38" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="3"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="5"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C52" s="5"/>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C54" s="5"/>
+      <c r="C54" s="3"/>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="5"/>
+      <c r="C56" s="3"/>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C57" s="5"/>
+      <c r="C57" s="3"/>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C58" s="4"/>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="4"/>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C60" s="4"/>
+      <c r="C60" s="2"/>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C61" s="4"/>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C62" s="4"/>
+      <c r="C62" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Hoan tat cap nhat theo file 27/09
Chuyen thoi gian nhac nho thanh 1p  1lan, cac moc tgian 5-15-20-25-30. Dieu chinh am luong khong phat am nua ma dieu chinh luon
</commit_message>
<xml_diff>
--- a/NewAudio/Audio.xlsx
+++ b/NewAudio/Audio.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\NewAudio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RunningMachine\NewAudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974E9D6E-8E2E-48BB-840E-118C3E84DEAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,9 +352,6 @@
     <t>luôn giữ hơi thở đều để không ảnh hưởng đến nhịp tim , nếu bạn cảm thấy mệt, hơi thở gấp hãy ấn nút speed trừ để giảm tốc độ cho phù hợp</t>
   </si>
   <si>
-    <t>Sau 5 phút đầu tiên, cứ 2 phút nhắc 1 lần</t>
-  </si>
-  <si>
     <t>Sau khi lắp lại khóa an toàn</t>
   </si>
   <si>
@@ -365,9 +361,6 @@
     <t>Khi tháo khóa an toàn</t>
   </si>
   <si>
-    <t>5 phút đầu tiên, nhắc tăng tốc sau 30s</t>
-  </si>
-  <si>
     <t>037</t>
   </si>
   <si>
@@ -375,12 +368,18 @@
   </si>
   <si>
     <t>Bạn hãy ấn nút Speed cộng để tăng dần tốc độ, nên bước đều chân ,thẳng lưng, mắt nhìn thẳng hướng về phía trước,lấy hơi thở đều để không ảnh hưởng đến nhịp tim, nếu bạn cảm thấy mệt, hơi thở gấp hãy ấn nút speed trừ để giảm tốc độ cho phù hợp</t>
+  </si>
+  <si>
+    <t>Sau 5 phút đầu tiên, cứ 2 phút nhắc 1 lần -&gt; 1p 1 lần</t>
+  </si>
+  <si>
+    <t>5 phút đầu tiên, nhắc tăng tốc sau 1p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -766,27 +765,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" style="4" customWidth="1"/>
     <col min="5" max="5" width="38" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="81.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="24.453125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="81.54296875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -809,7 +808,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="406" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -832,7 +831,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="375" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -852,7 +851,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -863,7 +862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -874,7 +873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -885,7 +884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -896,7 +895,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -916,7 +915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -927,7 +926,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -938,7 +937,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -949,7 +948,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -960,7 +959,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -971,7 +970,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -982,7 +981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -993,7 +992,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1004,7 +1003,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1037,12 +1036,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>21</v>
@@ -1060,7 +1059,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1115,7 +1114,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1154,7 +1153,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1165,12 +1164,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>60</v>
@@ -1179,12 +1178,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>63</v>
@@ -1196,12 +1195,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="261" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>64</v>
@@ -1216,7 +1215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1233,7 +1232,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1282,100 +1281,100 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>86</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C39" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update khong nhac nho khi chay voi bai tap mac dinh
</commit_message>
<xml_diff>
--- a/NewAudio/Audio.xlsx
+++ b/NewAudio/Audio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RunningMachine\NewAudio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PJ5\RunningMachine\NewAudio\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D51A719-FB78-4AB7-B1A7-81B722299CA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -375,11 +376,14 @@
   <si>
     <t>5 phút đầu tiên, nhắc tăng tốc sau 1p</t>
   </si>
+  <si>
+    <t>Bạn đang luyện tập với bài tập mặc định, chú ý giữ an toàn khi máy thay đổi độ dốc và tốc độ nhé</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -484,6 +488,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,27 +772,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7265625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.453125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="81.54296875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="81.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="83.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -807,8 +815,11 @@
       <c r="G1" s="15" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="406" x14ac:dyDescent="0.35">
+      <c r="H1" s="16">
+        <v>44114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -831,7 +842,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="375" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -851,7 +862,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -862,7 +873,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -873,7 +884,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -884,7 +895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -895,7 +906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -915,7 +926,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -926,7 +937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -937,7 +948,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -948,7 +959,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -959,7 +970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -970,7 +981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -981,7 +992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -992,7 +1003,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1003,7 +1014,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1014,7 +1025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1025,7 +1036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1036,7 +1047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1059,7 +1070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1070,7 +1081,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1081,7 +1092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1092,7 +1103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1103,7 +1114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1114,7 +1125,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1136,7 +1147,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1153,7 +1164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1164,7 +1175,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1178,7 +1189,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1195,7 +1206,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="261" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="270" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1232,7 +1243,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1249,7 +1260,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1281,7 +1292,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1295,86 +1306,89 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
     </row>
   </sheetData>

</xml_diff>